<commit_message>
added reactive power and generators to the analysis
</commit_message>
<xml_diff>
--- a/grids/ct217_grid_model_v0.2.xlsx
+++ b/grids/ct217_grid_model_v0.2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\CITCEA.PRJ_220_UnicoCloud_PLATON\06. documentacio tecnica\PilotData\CT-0217\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinicius\Google Drive\PycharmProjects\congestion-application\grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="161">
   <si>
     <t>x</t>
   </si>
@@ -606,33 +606,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1003,10 +998,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1034,7 +1029,7 @@
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>56</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1045,48 +1040,48 @@
       <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="4">
         <v>5.25</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="3"/>
       <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <v>0.23</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="3"/>
       <c r="F3" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <v>0.23</v>
       </c>
       <c r="D4" t="s">
@@ -1100,10 +1095,10 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>0.23</v>
       </c>
       <c r="D5" t="s">
@@ -1117,10 +1112,10 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>0.23</v>
       </c>
       <c r="D6" t="s">
@@ -1134,10 +1129,10 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7">
         <v>0.23</v>
       </c>
       <c r="D7" t="s">
@@ -1151,10 +1146,10 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8">
         <v>0.23</v>
       </c>
       <c r="D8" t="s">
@@ -1168,10 +1163,10 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>7</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9">
         <v>0.23</v>
       </c>
       <c r="D9" t="s">
@@ -1185,10 +1180,10 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10">
         <v>8</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10">
         <v>0.23</v>
       </c>
       <c r="D10" t="s">
@@ -1202,10 +1197,10 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11">
         <v>9</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11">
         <v>0.23</v>
       </c>
       <c r="D11" t="s">
@@ -1219,10 +1214,10 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12">
         <v>10</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12">
         <v>0.23</v>
       </c>
       <c r="D12" t="s">
@@ -1236,10 +1231,10 @@
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13">
         <v>11</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13">
         <v>0.23</v>
       </c>
       <c r="D13" t="s">
@@ -1253,10 +1248,10 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14">
         <v>12</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14">
         <v>0.23</v>
       </c>
       <c r="D14" t="s">
@@ -1270,10 +1265,10 @@
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15">
         <v>13</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15">
         <v>0.23</v>
       </c>
       <c r="D15" t="s">
@@ -1287,10 +1282,10 @@
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16">
         <v>14</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16">
         <v>0.23</v>
       </c>
       <c r="D16" t="s">
@@ -1307,13 +1302,13 @@
       <c r="B17">
         <v>81985</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17">
         <v>0.23</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17">
         <v>2</v>
       </c>
       <c r="F17" t="b">
@@ -1330,13 +1325,13 @@
       <c r="B18">
         <v>82133</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18">
         <v>0.23</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18">
         <v>2</v>
       </c>
       <c r="F18" t="b">
@@ -1353,13 +1348,13 @@
       <c r="B19">
         <v>82769</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19">
         <v>0.23</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19">
         <v>2</v>
       </c>
       <c r="F19" t="b">
@@ -1376,13 +1371,13 @@
       <c r="B20">
         <v>86136</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20">
         <v>0.23</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20">
         <v>1</v>
       </c>
       <c r="F20" t="b">
@@ -1399,13 +1394,13 @@
       <c r="B21">
         <v>86139</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21">
         <v>0.23</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21">
         <v>1</v>
       </c>
       <c r="F21" t="b">
@@ -1422,13 +1417,13 @@
       <c r="B22">
         <v>86192</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22">
         <v>0.23</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22">
         <v>1</v>
       </c>
       <c r="F22" t="b">
@@ -1445,13 +1440,13 @@
       <c r="B23">
         <v>87953</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23">
         <v>0.23</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23">
         <v>2</v>
       </c>
       <c r="F23" t="b">
@@ -1468,13 +1463,13 @@
       <c r="B24">
         <v>88124</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24">
         <v>0.23</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24">
         <v>2</v>
       </c>
       <c r="F24" t="b">
@@ -1491,13 +1486,13 @@
       <c r="B25">
         <v>88652</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25">
         <v>0.23</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25">
         <v>2</v>
       </c>
       <c r="F25" t="b">
@@ -1514,13 +1509,13 @@
       <c r="B26">
         <v>90335</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26">
         <v>0.23</v>
       </c>
       <c r="D26" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26">
         <v>2</v>
       </c>
       <c r="F26" t="b">
@@ -1537,13 +1532,13 @@
       <c r="B27">
         <v>90410</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27">
         <v>0.23</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27">
         <v>1</v>
       </c>
       <c r="F27" t="b">
@@ -1560,13 +1555,13 @@
       <c r="B28">
         <v>90629</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28">
         <v>0.23</v>
       </c>
       <c r="D28" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28">
         <v>1</v>
       </c>
       <c r="F28" t="b">
@@ -1583,13 +1578,13 @@
       <c r="B29">
         <v>91440</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29">
         <v>0.23</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29">
         <v>1</v>
       </c>
       <c r="F29" t="b">
@@ -1606,13 +1601,13 @@
       <c r="B30">
         <v>91648</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30">
         <v>0.23</v>
       </c>
       <c r="D30" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30">
         <v>1</v>
       </c>
       <c r="F30" t="b">
@@ -1629,13 +1624,13 @@
       <c r="B31">
         <v>93353</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31">
         <v>0.23</v>
       </c>
       <c r="D31" t="s">
         <v>9</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31">
         <v>3</v>
       </c>
       <c r="F31" t="b">
@@ -1652,13 +1647,13 @@
       <c r="B32">
         <v>94117</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32">
         <v>0.23</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32">
         <v>2</v>
       </c>
       <c r="F32" t="b">
@@ -1675,13 +1670,13 @@
       <c r="B33">
         <v>94130</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33">
         <v>0.23</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33">
         <v>3</v>
       </c>
       <c r="F33" t="b">
@@ -1698,13 +1693,13 @@
       <c r="B34">
         <v>96061</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34">
         <v>0.23</v>
       </c>
       <c r="D34" t="s">
         <v>9</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34">
         <v>5</v>
       </c>
       <c r="F34" t="b">
@@ -1721,13 +1716,13 @@
       <c r="B35">
         <v>97390</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35">
         <v>0.23</v>
       </c>
       <c r="D35" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35">
         <v>2</v>
       </c>
       <c r="F35" t="b">
@@ -1744,13 +1739,13 @@
       <c r="B36">
         <v>98806</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36">
         <v>0.23</v>
       </c>
       <c r="D36" t="s">
         <v>9</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36">
         <v>3</v>
       </c>
       <c r="F36" t="b">
@@ -1767,13 +1762,13 @@
       <c r="B37">
         <v>99374</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37">
         <v>0.23</v>
       </c>
       <c r="D37" t="s">
         <v>9</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37">
         <v>3</v>
       </c>
       <c r="F37" t="b">
@@ -1790,13 +1785,13 @@
       <c r="B38">
         <v>101145</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38">
         <v>0.23</v>
       </c>
       <c r="D38" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38">
         <v>1</v>
       </c>
       <c r="F38" t="b">
@@ -1813,13 +1808,13 @@
       <c r="B39">
         <v>108024</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39">
         <v>0.23</v>
       </c>
       <c r="D39" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39">
         <v>1</v>
       </c>
       <c r="F39" t="b">
@@ -1836,13 +1831,13 @@
       <c r="B40">
         <v>120604</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40">
         <v>0.23</v>
       </c>
       <c r="D40" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40">
         <v>1</v>
       </c>
       <c r="F40" t="b">
@@ -1859,13 +1854,13 @@
       <c r="B41">
         <v>123294</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41">
         <v>0.23</v>
       </c>
       <c r="D41" t="s">
         <v>9</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41">
         <v>3</v>
       </c>
       <c r="F41" t="b">
@@ -1882,13 +1877,13 @@
       <c r="B42">
         <v>127923</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42">
         <v>0.23</v>
       </c>
       <c r="D42" t="s">
         <v>9</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42">
         <v>1</v>
       </c>
       <c r="F42" t="b">
@@ -1905,13 +1900,13 @@
       <c r="B43">
         <v>129965</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43">
         <v>0.23</v>
       </c>
       <c r="D43" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43">
         <v>1</v>
       </c>
       <c r="F43" t="b">
@@ -1928,13 +1923,13 @@
       <c r="B44">
         <v>131793</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44">
         <v>0.23</v>
       </c>
       <c r="D44" t="s">
         <v>9</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44">
         <v>1</v>
       </c>
       <c r="F44" t="b">
@@ -1951,13 +1946,13 @@
       <c r="B45">
         <v>135493</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45">
         <v>0.23</v>
       </c>
       <c r="D45" t="s">
         <v>9</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45">
         <v>2</v>
       </c>
       <c r="F45" t="b">
@@ -1974,8 +1969,11 @@
       <c r="B46">
         <v>44</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46">
         <v>0.23</v>
+      </c>
+      <c r="D46" t="s">
+        <v>9</v>
       </c>
       <c r="F46" t="b">
         <v>1</v>
@@ -1988,10 +1986,30 @@
       <c r="B47">
         <v>45</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47">
         <v>0.23</v>
       </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
       <c r="F47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <v>46</v>
+      </c>
+      <c r="C48">
+        <v>0.23</v>
+      </c>
+      <c r="D48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2006,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43:P43"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2099,7 @@
       <c r="B2">
         <v>6016</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" t="s">
         <v>59</v>
       </c>
       <c r="D2">
@@ -2093,25 +2111,25 @@
       <c r="F2">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="7">
         <v>0.16</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="7">
         <v>0.18</v>
       </c>
-      <c r="I2" s="12">
+      <c r="I2" s="9">
         <v>11</v>
       </c>
-      <c r="J2" s="9">
-        <v>0</v>
-      </c>
-      <c r="K2" s="9">
+      <c r="J2" s="7">
+        <v>0</v>
+      </c>
+      <c r="K2" s="7">
         <v>0.34399999999999997</v>
       </c>
-      <c r="L2" s="9">
-        <v>1</v>
-      </c>
-      <c r="M2" s="9">
+      <c r="L2" s="7">
+        <v>1</v>
+      </c>
+      <c r="M2" s="7">
         <v>1</v>
       </c>
       <c r="N2" t="s">
@@ -2128,7 +2146,7 @@
       <c r="B3">
         <v>6026</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" t="s">
         <v>60</v>
       </c>
       <c r="D3">
@@ -2140,25 +2158,25 @@
       <c r="F3">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="9">
         <v>0.30599999999999999</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="9">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="9">
         <v>13.2</v>
       </c>
-      <c r="J3" s="9">
-        <v>0</v>
-      </c>
-      <c r="K3" s="9">
+      <c r="J3" s="7">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
         <v>0.23</v>
       </c>
-      <c r="L3" s="9">
-        <v>1</v>
-      </c>
-      <c r="M3" s="9">
+      <c r="L3" s="7">
+        <v>1</v>
+      </c>
+      <c r="M3" s="7">
         <v>1</v>
       </c>
       <c r="N3" t="s">
@@ -2175,7 +2193,7 @@
       <c r="B4">
         <v>121290</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" t="s">
         <v>60</v>
       </c>
       <c r="D4">
@@ -2187,25 +2205,25 @@
       <c r="F4">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="9">
         <v>0.30599999999999999</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="9">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="9">
         <v>13.2</v>
       </c>
-      <c r="J4" s="9">
-        <v>0</v>
-      </c>
-      <c r="K4" s="9">
+      <c r="J4" s="7">
+        <v>0</v>
+      </c>
+      <c r="K4" s="7">
         <v>0.23</v>
       </c>
-      <c r="L4" s="9">
-        <v>1</v>
-      </c>
-      <c r="M4" s="9">
+      <c r="L4" s="7">
+        <v>1</v>
+      </c>
+      <c r="M4" s="7">
         <v>1</v>
       </c>
       <c r="N4" t="s">
@@ -2222,7 +2240,7 @@
       <c r="B5">
         <v>6028</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" t="s">
         <v>62</v>
       </c>
       <c r="D5">
@@ -2234,25 +2252,25 @@
       <c r="F5">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>1.43</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="9">
         <v>11</v>
       </c>
-      <c r="J5" s="9">
-        <v>0</v>
-      </c>
-      <c r="K5" s="9">
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L5" s="9">
-        <v>1</v>
-      </c>
-      <c r="M5" s="9">
+      <c r="L5" s="7">
+        <v>1</v>
+      </c>
+      <c r="M5" s="7">
         <v>1</v>
       </c>
       <c r="N5" t="s">
@@ -2266,10 +2284,10 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" t="s">
         <v>60</v>
       </c>
       <c r="D6">
@@ -2281,25 +2299,25 @@
       <c r="F6">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="9">
         <v>0.30599999999999999</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="9">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="9">
         <v>13.2</v>
       </c>
-      <c r="J6" s="9">
-        <v>0</v>
-      </c>
-      <c r="K6" s="9">
+      <c r="J6" s="7">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
         <v>0.23</v>
       </c>
-      <c r="L6" s="9">
-        <v>1</v>
-      </c>
-      <c r="M6" s="9">
+      <c r="L6" s="7">
+        <v>1</v>
+      </c>
+      <c r="M6" s="7">
         <v>1</v>
       </c>
       <c r="N6" t="s">
@@ -2319,7 +2337,7 @@
       <c r="B7">
         <v>6030</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" t="s">
         <v>63</v>
       </c>
       <c r="D7">
@@ -2331,25 +2349,25 @@
       <c r="F7">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="7">
         <v>1.43</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="9">
         <v>11</v>
       </c>
-      <c r="J7" s="9">
-        <v>0</v>
-      </c>
-      <c r="K7" s="9">
+      <c r="J7" s="7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L7" s="9">
-        <v>1</v>
-      </c>
-      <c r="M7" s="9">
+      <c r="L7" s="7">
+        <v>1</v>
+      </c>
+      <c r="M7" s="7">
         <v>1</v>
       </c>
       <c r="N7" t="s">
@@ -2363,10 +2381,10 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" t="s">
         <v>64</v>
       </c>
       <c r="D8">
@@ -2378,25 +2396,25 @@
       <c r="F8">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="7">
         <v>0.90700000000000003</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="9">
         <v>11.25</v>
       </c>
-      <c r="J8" s="9">
-        <v>0</v>
-      </c>
-      <c r="K8" s="9">
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
         <v>0.128</v>
       </c>
-      <c r="L8" s="9">
-        <v>1</v>
-      </c>
-      <c r="M8" s="9">
+      <c r="L8" s="7">
+        <v>1</v>
+      </c>
+      <c r="M8" s="7">
         <v>1</v>
       </c>
       <c r="N8" t="s">
@@ -2416,7 +2434,7 @@
       <c r="B9">
         <v>6018</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" t="s">
         <v>63</v>
       </c>
       <c r="D9">
@@ -2428,25 +2446,25 @@
       <c r="F9">
         <v>3.1E-2</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>1.43</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="9">
         <v>11</v>
       </c>
-      <c r="J9" s="9">
-        <v>0</v>
-      </c>
-      <c r="K9" s="9">
+      <c r="J9" s="7">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L9" s="9">
-        <v>1</v>
-      </c>
-      <c r="M9" s="9">
+      <c r="L9" s="7">
+        <v>1</v>
+      </c>
+      <c r="M9" s="7">
         <v>1</v>
       </c>
       <c r="N9" t="s">
@@ -2460,10 +2478,10 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" t="s">
         <v>60</v>
       </c>
       <c r="D10">
@@ -2475,25 +2493,25 @@
       <c r="F10">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="9">
         <v>0.30599999999999999</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="9">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="9">
         <v>13.2</v>
       </c>
-      <c r="J10" s="9">
-        <v>0</v>
-      </c>
-      <c r="K10" s="9">
+      <c r="J10" s="7">
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
         <v>0.23</v>
       </c>
-      <c r="L10" s="9">
-        <v>1</v>
-      </c>
-      <c r="M10" s="9">
+      <c r="L10" s="7">
+        <v>1</v>
+      </c>
+      <c r="M10" s="7">
         <v>1</v>
       </c>
       <c r="N10" t="s">
@@ -2510,7 +2528,7 @@
       <c r="B11">
         <v>6020</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" t="s">
         <v>63</v>
       </c>
       <c r="D11">
@@ -2522,25 +2540,25 @@
       <c r="F11">
         <v>1.9E-2</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="7">
         <v>1.43</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="9">
         <v>11</v>
       </c>
-      <c r="J11" s="9">
-        <v>0</v>
-      </c>
-      <c r="K11" s="9">
+      <c r="J11" s="7">
+        <v>0</v>
+      </c>
+      <c r="K11" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L11" s="9">
-        <v>1</v>
-      </c>
-      <c r="M11" s="9">
+      <c r="L11" s="7">
+        <v>1</v>
+      </c>
+      <c r="M11" s="7">
         <v>1</v>
       </c>
       <c r="N11" t="s">
@@ -2560,7 +2578,7 @@
       <c r="B12">
         <v>121294</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" t="s">
         <v>60</v>
       </c>
       <c r="D12">
@@ -2572,25 +2590,25 @@
       <c r="F12">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="9">
         <v>0.30599999999999999</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="9">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="9">
         <v>13.2</v>
       </c>
-      <c r="J12" s="9">
-        <v>0</v>
-      </c>
-      <c r="K12" s="9">
+      <c r="J12" s="7">
+        <v>0</v>
+      </c>
+      <c r="K12" s="7">
         <v>0.23</v>
       </c>
-      <c r="L12" s="9">
-        <v>1</v>
-      </c>
-      <c r="M12" s="9">
+      <c r="L12" s="7">
+        <v>1</v>
+      </c>
+      <c r="M12" s="7">
         <v>1</v>
       </c>
       <c r="N12" t="s">
@@ -2607,7 +2625,7 @@
       <c r="B13">
         <v>6022</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" t="s">
         <v>62</v>
       </c>
       <c r="D13">
@@ -2619,25 +2637,25 @@
       <c r="F13">
         <v>0.02</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="7">
         <v>1.43</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="9">
         <v>11</v>
       </c>
-      <c r="J13" s="9">
-        <v>0</v>
-      </c>
-      <c r="K13" s="9">
+      <c r="J13" s="7">
+        <v>0</v>
+      </c>
+      <c r="K13" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L13" s="9">
-        <v>1</v>
-      </c>
-      <c r="M13" s="9">
+      <c r="L13" s="7">
+        <v>1</v>
+      </c>
+      <c r="M13" s="7">
         <v>1</v>
       </c>
       <c r="N13" t="s">
@@ -2654,7 +2672,7 @@
       <c r="B14">
         <v>6021</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" t="s">
         <v>65</v>
       </c>
       <c r="D14">
@@ -2666,25 +2684,25 @@
       <c r="F14">
         <v>3.9E-2</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="7">
         <v>1.43</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="9">
         <v>11</v>
       </c>
-      <c r="J14" s="9">
-        <v>0</v>
-      </c>
-      <c r="K14" s="9">
+      <c r="J14" s="7">
+        <v>0</v>
+      </c>
+      <c r="K14" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L14" s="9">
-        <v>1</v>
-      </c>
-      <c r="M14" s="9">
+      <c r="L14" s="7">
+        <v>1</v>
+      </c>
+      <c r="M14" s="7">
         <v>1</v>
       </c>
       <c r="N14" t="s">
@@ -2701,7 +2719,7 @@
       <c r="B15">
         <v>121293</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" t="s">
         <v>60</v>
       </c>
       <c r="D15">
@@ -2713,25 +2731,25 @@
       <c r="F15">
         <v>3.1E-2</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="9">
         <v>0.30599999999999999</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="9">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="9">
         <v>13.2</v>
       </c>
-      <c r="J15" s="9">
-        <v>0</v>
-      </c>
-      <c r="K15" s="9">
+      <c r="J15" s="7">
+        <v>0</v>
+      </c>
+      <c r="K15" s="7">
         <v>0.23</v>
       </c>
-      <c r="L15" s="9">
-        <v>1</v>
-      </c>
-      <c r="M15" s="9">
+      <c r="L15" s="7">
+        <v>1</v>
+      </c>
+      <c r="M15" s="7">
         <v>1</v>
       </c>
       <c r="N15" t="s">
@@ -2748,10 +2766,10 @@
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" t="s">
         <v>63</v>
       </c>
       <c r="D16">
@@ -2763,25 +2781,25 @@
       <c r="F16">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="7">
         <v>1.43</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="9">
         <v>11</v>
       </c>
-      <c r="J16" s="9">
-        <v>0</v>
-      </c>
-      <c r="K16" s="9">
+      <c r="J16" s="7">
+        <v>0</v>
+      </c>
+      <c r="K16" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L16" s="9">
-        <v>1</v>
-      </c>
-      <c r="M16" s="9">
+      <c r="L16" s="7">
+        <v>1</v>
+      </c>
+      <c r="M16" s="7">
         <v>1</v>
       </c>
       <c r="N16" t="s">
@@ -2798,10 +2816,10 @@
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="8">
         <v>5999</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" t="s">
         <v>59</v>
       </c>
       <c r="D17">
@@ -2813,25 +2831,25 @@
       <c r="F17">
         <v>0.17599999999999999</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="7">
         <v>0.16</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="7">
         <v>0.18</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="9">
         <v>11</v>
       </c>
-      <c r="J17" s="9">
-        <v>0</v>
-      </c>
-      <c r="K17" s="9">
+      <c r="J17" s="7">
+        <v>0</v>
+      </c>
+      <c r="K17" s="7">
         <v>0.34399999999999997</v>
       </c>
-      <c r="L17" s="9">
-        <v>1</v>
-      </c>
-      <c r="M17" s="9">
+      <c r="L17" s="7">
+        <v>1</v>
+      </c>
+      <c r="M17" s="7">
         <v>1</v>
       </c>
       <c r="N17" t="s">
@@ -2845,10 +2863,10 @@
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="8">
         <v>121014</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" t="s">
         <v>59</v>
       </c>
       <c r="D18">
@@ -2860,25 +2878,25 @@
       <c r="F18">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="7">
         <v>0.16</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="7">
         <v>0.18</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="9">
         <v>11</v>
       </c>
-      <c r="J18" s="9">
-        <v>0</v>
-      </c>
-      <c r="K18" s="9">
+      <c r="J18" s="7">
+        <v>0</v>
+      </c>
+      <c r="K18" s="7">
         <v>0.34399999999999997</v>
       </c>
-      <c r="L18" s="9">
-        <v>1</v>
-      </c>
-      <c r="M18" s="9">
+      <c r="L18" s="7">
+        <v>1</v>
+      </c>
+      <c r="M18" s="7">
         <v>1</v>
       </c>
       <c r="N18" t="s">
@@ -2892,10 +2910,10 @@
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" t="s">
         <v>110</v>
       </c>
       <c r="D19">
@@ -2907,25 +2925,25 @@
       <c r="F19">
         <v>0.11</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="7">
         <v>0.82099999999999995</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="7">
         <v>0.223</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="9">
         <v>11</v>
       </c>
-      <c r="J19" s="9">
-        <v>0</v>
-      </c>
-      <c r="K19" s="9">
+      <c r="J19" s="7">
+        <v>0</v>
+      </c>
+      <c r="K19" s="7">
         <v>0.14399999999999999</v>
       </c>
-      <c r="L19" s="9">
-        <v>1</v>
-      </c>
-      <c r="M19" s="9">
+      <c r="L19" s="7">
+        <v>1</v>
+      </c>
+      <c r="M19" s="7">
         <v>1</v>
       </c>
       <c r="N19" t="s">
@@ -2942,10 +2960,10 @@
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" t="s">
         <v>59</v>
       </c>
       <c r="D20">
@@ -2957,25 +2975,25 @@
       <c r="F20">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="7">
         <v>0.16</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="7">
         <v>0.18</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="9">
         <v>11</v>
       </c>
-      <c r="J20" s="9">
-        <v>0</v>
-      </c>
-      <c r="K20" s="9">
+      <c r="J20" s="7">
+        <v>0</v>
+      </c>
+      <c r="K20" s="7">
         <v>0.34399999999999997</v>
       </c>
-      <c r="L20" s="9">
-        <v>1</v>
-      </c>
-      <c r="M20" s="9">
+      <c r="L20" s="7">
+        <v>1</v>
+      </c>
+      <c r="M20" s="7">
         <v>1</v>
       </c>
       <c r="N20" t="s">
@@ -2992,10 +3010,10 @@
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="8">
         <v>6008</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" t="s">
         <v>59</v>
       </c>
       <c r="D21">
@@ -3007,25 +3025,25 @@
       <c r="F21">
         <v>0.10299999999999999</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="7">
         <v>0.16</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="7">
         <v>0.18</v>
       </c>
-      <c r="I21" s="12">
+      <c r="I21" s="9">
         <v>11</v>
       </c>
-      <c r="J21" s="9">
-        <v>0</v>
-      </c>
-      <c r="K21" s="9">
+      <c r="J21" s="7">
+        <v>0</v>
+      </c>
+      <c r="K21" s="7">
         <v>0.34399999999999997</v>
       </c>
-      <c r="L21" s="9">
-        <v>1</v>
-      </c>
-      <c r="M21" s="9">
+      <c r="L21" s="7">
+        <v>1</v>
+      </c>
+      <c r="M21" s="7">
         <v>1</v>
       </c>
       <c r="N21" t="s">
@@ -3039,10 +3057,10 @@
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="8">
         <v>6010</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" t="s">
         <v>65</v>
       </c>
       <c r="D22">
@@ -3054,25 +3072,25 @@
       <c r="F22">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="7">
         <v>1.43</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="9">
         <v>11</v>
       </c>
-      <c r="J22" s="9">
-        <v>0</v>
-      </c>
-      <c r="K22" s="9">
+      <c r="J22" s="7">
+        <v>0</v>
+      </c>
+      <c r="K22" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L22" s="9">
-        <v>1</v>
-      </c>
-      <c r="M22" s="9">
+      <c r="L22" s="7">
+        <v>1</v>
+      </c>
+      <c r="M22" s="7">
         <v>1</v>
       </c>
       <c r="N22" t="s">
@@ -3086,10 +3104,10 @@
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="8">
         <v>6009</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" t="s">
         <v>65</v>
       </c>
       <c r="D23">
@@ -3101,25 +3119,25 @@
       <c r="F23">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="7">
         <v>1.43</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I23" s="12">
+      <c r="I23" s="9">
         <v>11</v>
       </c>
-      <c r="J23" s="9">
-        <v>0</v>
-      </c>
-      <c r="K23" s="9">
+      <c r="J23" s="7">
+        <v>0</v>
+      </c>
+      <c r="K23" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L23" s="9">
-        <v>1</v>
-      </c>
-      <c r="M23" s="9">
+      <c r="L23" s="7">
+        <v>1</v>
+      </c>
+      <c r="M23" s="7">
         <v>1</v>
       </c>
       <c r="N23" t="s">
@@ -3133,10 +3151,10 @@
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="8">
         <v>6011</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" t="s">
         <v>62</v>
       </c>
       <c r="D24">
@@ -3148,25 +3166,25 @@
       <c r="F24">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="7">
         <v>1.43</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I24" s="12">
+      <c r="I24" s="9">
         <v>11</v>
       </c>
-      <c r="J24" s="9">
-        <v>0</v>
-      </c>
-      <c r="K24" s="9">
+      <c r="J24" s="7">
+        <v>0</v>
+      </c>
+      <c r="K24" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L24" s="9">
-        <v>1</v>
-      </c>
-      <c r="M24" s="9">
+      <c r="L24" s="7">
+        <v>1</v>
+      </c>
+      <c r="M24" s="7">
         <v>1</v>
       </c>
       <c r="N24" t="s">
@@ -3180,10 +3198,10 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="8">
         <v>6012</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" t="s">
         <v>59</v>
       </c>
       <c r="D25">
@@ -3195,25 +3213,25 @@
       <c r="F25">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="7">
         <v>0.16</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="7">
         <v>0.18</v>
       </c>
-      <c r="I25" s="12">
+      <c r="I25" s="9">
         <v>11</v>
       </c>
-      <c r="J25" s="9">
-        <v>0</v>
-      </c>
-      <c r="K25" s="9">
+      <c r="J25" s="7">
+        <v>0</v>
+      </c>
+      <c r="K25" s="7">
         <v>0.34399999999999997</v>
       </c>
-      <c r="L25" s="9">
-        <v>1</v>
-      </c>
-      <c r="M25" s="9">
+      <c r="L25" s="7">
+        <v>1</v>
+      </c>
+      <c r="M25" s="7">
         <v>1</v>
       </c>
       <c r="N25" t="s">
@@ -3227,10 +3245,10 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="8">
         <v>6014</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" t="s">
         <v>62</v>
       </c>
       <c r="D26">
@@ -3242,25 +3260,25 @@
       <c r="F26">
         <v>1E-3</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="7">
         <v>1.43</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I26" s="12">
+      <c r="I26" s="9">
         <v>11</v>
       </c>
-      <c r="J26" s="9">
-        <v>0</v>
-      </c>
-      <c r="K26" s="9">
+      <c r="J26" s="7">
+        <v>0</v>
+      </c>
+      <c r="K26" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L26" s="9">
-        <v>1</v>
-      </c>
-      <c r="M26" s="9">
+      <c r="L26" s="7">
+        <v>1</v>
+      </c>
+      <c r="M26" s="7">
         <v>1</v>
       </c>
       <c r="N26" t="s">
@@ -3274,10 +3292,10 @@
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="8">
         <v>6015</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" t="s">
         <v>99</v>
       </c>
       <c r="D27">
@@ -3289,25 +3307,25 @@
       <c r="F27">
         <v>0.01</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="7">
         <v>2.27</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="I27" s="12">
+      <c r="I27" s="9">
         <v>11</v>
       </c>
-      <c r="J27" s="9">
-        <v>0</v>
-      </c>
-      <c r="K27" s="9">
+      <c r="J27" s="7">
+        <v>0</v>
+      </c>
+      <c r="K27" s="7">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="L27" s="9">
-        <v>1</v>
-      </c>
-      <c r="M27" s="9">
+      <c r="L27" s="7">
+        <v>1</v>
+      </c>
+      <c r="M27" s="7">
         <v>1</v>
       </c>
       <c r="N27" t="s">
@@ -3321,10 +3339,10 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="8">
         <v>6013</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" t="s">
         <v>62</v>
       </c>
       <c r="D28">
@@ -3336,25 +3354,25 @@
       <c r="F28">
         <v>1.2E-2</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="7">
         <v>1.43</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I28" s="12">
+      <c r="I28" s="9">
         <v>11</v>
       </c>
-      <c r="J28" s="9">
-        <v>0</v>
-      </c>
-      <c r="K28" s="9">
+      <c r="J28" s="7">
+        <v>0</v>
+      </c>
+      <c r="K28" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L28" s="9">
-        <v>1</v>
-      </c>
-      <c r="M28" s="9">
+      <c r="L28" s="7">
+        <v>1</v>
+      </c>
+      <c r="M28" s="7">
         <v>1</v>
       </c>
       <c r="N28" t="s">
@@ -3368,10 +3386,10 @@
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="8">
         <v>6000</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" t="s">
         <v>62</v>
       </c>
       <c r="D29">
@@ -3383,25 +3401,25 @@
       <c r="F29">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="7">
         <v>1.43</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I29" s="12">
+      <c r="I29" s="9">
         <v>11</v>
       </c>
-      <c r="J29" s="9">
-        <v>0</v>
-      </c>
-      <c r="K29" s="9">
+      <c r="J29" s="7">
+        <v>0</v>
+      </c>
+      <c r="K29" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L29" s="9">
-        <v>1</v>
-      </c>
-      <c r="M29" s="9">
+      <c r="L29" s="7">
+        <v>1</v>
+      </c>
+      <c r="M29" s="7">
         <v>1</v>
       </c>
       <c r="N29" t="s">
@@ -3415,7 +3433,7 @@
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="8">
         <v>6001</v>
       </c>
       <c r="C30" t="s">
@@ -3430,25 +3448,25 @@
       <c r="F30">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="7">
         <v>0.41</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="7">
         <v>0.20499999999999999</v>
       </c>
-      <c r="I30" s="12">
+      <c r="I30" s="9">
         <v>13.2</v>
       </c>
-      <c r="J30" s="9">
-        <v>0</v>
-      </c>
-      <c r="K30" s="9">
+      <c r="J30" s="7">
+        <v>0</v>
+      </c>
+      <c r="K30" s="7">
         <v>0.20799999999999999</v>
       </c>
-      <c r="L30" s="9">
-        <v>1</v>
-      </c>
-      <c r="M30" s="9">
+      <c r="L30" s="7">
+        <v>1</v>
+      </c>
+      <c r="M30" s="7">
         <v>1</v>
       </c>
       <c r="N30" t="s">
@@ -3462,10 +3480,10 @@
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="8">
         <v>6002</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" t="s">
         <v>65</v>
       </c>
       <c r="D31">
@@ -3477,25 +3495,25 @@
       <c r="F31">
         <v>0.04</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="7">
         <v>1.43</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H31" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I31" s="12">
+      <c r="I31" s="9">
         <v>11</v>
       </c>
-      <c r="J31" s="9">
-        <v>0</v>
-      </c>
-      <c r="K31" s="9">
+      <c r="J31" s="7">
+        <v>0</v>
+      </c>
+      <c r="K31" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L31" s="9">
-        <v>1</v>
-      </c>
-      <c r="M31" s="9">
+      <c r="L31" s="7">
+        <v>1</v>
+      </c>
+      <c r="M31" s="7">
         <v>1</v>
       </c>
       <c r="N31" t="s">
@@ -3509,10 +3527,10 @@
       <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="8">
         <v>6003</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" t="s">
         <v>100</v>
       </c>
       <c r="D32">
@@ -3524,25 +3542,25 @@
       <c r="F32">
         <v>6.3E-2</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="7">
         <v>1.1120000000000001</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="7">
         <v>0.23200000000000001</v>
       </c>
-      <c r="I32" s="12">
+      <c r="I32" s="9">
         <v>11</v>
       </c>
-      <c r="J32" s="9">
-        <v>0</v>
-      </c>
-      <c r="K32" s="9">
+      <c r="J32" s="7">
+        <v>0</v>
+      </c>
+      <c r="K32" s="7">
         <v>0.12</v>
       </c>
-      <c r="L32" s="9">
-        <v>1</v>
-      </c>
-      <c r="M32" s="9">
+      <c r="L32" s="7">
+        <v>1</v>
+      </c>
+      <c r="M32" s="7">
         <v>1</v>
       </c>
       <c r="N32" t="s">
@@ -3556,10 +3574,10 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="8">
         <v>6004</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" t="s">
         <v>65</v>
       </c>
       <c r="D33">
@@ -3571,25 +3589,25 @@
       <c r="F33">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="7">
         <v>1.43</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H33" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I33" s="12">
+      <c r="I33" s="9">
         <v>11</v>
       </c>
-      <c r="J33" s="9">
-        <v>0</v>
-      </c>
-      <c r="K33" s="9">
+      <c r="J33" s="7">
+        <v>0</v>
+      </c>
+      <c r="K33" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L33" s="9">
-        <v>1</v>
-      </c>
-      <c r="M33" s="9">
+      <c r="L33" s="7">
+        <v>1</v>
+      </c>
+      <c r="M33" s="7">
         <v>1</v>
       </c>
       <c r="N33" t="s">
@@ -3603,10 +3621,10 @@
       <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B34" s="8">
         <v>6005</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" t="s">
         <v>101</v>
       </c>
       <c r="D34">
@@ -3618,25 +3636,25 @@
       <c r="F34">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="G34" s="9">
+      <c r="G34" s="7">
         <v>2.27</v>
       </c>
-      <c r="H34" s="9">
+      <c r="H34" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="I34" s="12">
+      <c r="I34" s="9">
         <v>11</v>
       </c>
-      <c r="J34" s="9">
-        <v>0</v>
-      </c>
-      <c r="K34" s="9">
+      <c r="J34" s="7">
+        <v>0</v>
+      </c>
+      <c r="K34" s="7">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="L34" s="9">
-        <v>1</v>
-      </c>
-      <c r="M34" s="9">
+      <c r="L34" s="7">
+        <v>1</v>
+      </c>
+      <c r="M34" s="7">
         <v>1</v>
       </c>
       <c r="N34" t="s">
@@ -3650,10 +3668,10 @@
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B35" s="8">
         <v>6006</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" t="s">
         <v>102</v>
       </c>
       <c r="D35">
@@ -3665,25 +3683,25 @@
       <c r="F35">
         <v>2.3E-2</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="7">
         <v>0.48299999999999998</v>
       </c>
-      <c r="H35" s="9">
+      <c r="H35" s="7">
         <v>7.8E-2</v>
       </c>
-      <c r="I35" s="12">
+      <c r="I35" s="9">
         <v>11</v>
       </c>
-      <c r="J35" s="9">
-        <v>0</v>
-      </c>
-      <c r="K35" s="9">
+      <c r="J35" s="7">
+        <v>0</v>
+      </c>
+      <c r="K35" s="7">
         <v>0.184</v>
       </c>
-      <c r="L35" s="9">
-        <v>1</v>
-      </c>
-      <c r="M35" s="9">
+      <c r="L35" s="7">
+        <v>1</v>
+      </c>
+      <c r="M35" s="7">
         <v>1</v>
       </c>
       <c r="N35" t="s">
@@ -3697,10 +3715,10 @@
       <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="8">
         <v>6007</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" t="s">
         <v>62</v>
       </c>
       <c r="D36">
@@ -3712,25 +3730,25 @@
       <c r="F36">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="7">
         <v>1.43</v>
       </c>
-      <c r="H36" s="9">
+      <c r="H36" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I36" s="12">
+      <c r="I36" s="9">
         <v>11</v>
       </c>
-      <c r="J36" s="9">
-        <v>0</v>
-      </c>
-      <c r="K36" s="9">
+      <c r="J36" s="7">
+        <v>0</v>
+      </c>
+      <c r="K36" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L36" s="9">
-        <v>1</v>
-      </c>
-      <c r="M36" s="9">
+      <c r="L36" s="7">
+        <v>1</v>
+      </c>
+      <c r="M36" s="7">
         <v>1</v>
       </c>
       <c r="N36" t="s">
@@ -3744,10 +3762,10 @@
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B37" s="8">
         <v>5998</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" t="s">
         <v>102</v>
       </c>
       <c r="D37">
@@ -3759,25 +3777,25 @@
       <c r="F37">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="7">
         <v>0.48299999999999998</v>
       </c>
-      <c r="H37" s="9">
+      <c r="H37" s="7">
         <v>7.8E-2</v>
       </c>
-      <c r="I37" s="12">
+      <c r="I37" s="9">
         <v>11</v>
       </c>
-      <c r="J37" s="9">
-        <v>0</v>
-      </c>
-      <c r="K37" s="9">
+      <c r="J37" s="7">
+        <v>0</v>
+      </c>
+      <c r="K37" s="7">
         <v>0.184</v>
       </c>
-      <c r="L37" s="9">
-        <v>1</v>
-      </c>
-      <c r="M37" s="9">
+      <c r="L37" s="7">
+        <v>1</v>
+      </c>
+      <c r="M37" s="7">
         <v>1</v>
       </c>
       <c r="N37" t="s">
@@ -3791,10 +3809,10 @@
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" t="s">
         <v>59</v>
       </c>
       <c r="D38">
@@ -3806,25 +3824,25 @@
       <c r="F38">
         <v>0.185</v>
       </c>
-      <c r="G38" s="9">
+      <c r="G38" s="7">
         <v>0.16</v>
       </c>
-      <c r="H38" s="9">
+      <c r="H38" s="7">
         <v>0.18</v>
       </c>
-      <c r="I38" s="12">
+      <c r="I38" s="9">
         <v>11</v>
       </c>
-      <c r="J38" s="9">
-        <v>0</v>
-      </c>
-      <c r="K38" s="9">
+      <c r="J38" s="7">
+        <v>0</v>
+      </c>
+      <c r="K38" s="7">
         <v>0.34399999999999997</v>
       </c>
-      <c r="L38" s="9">
-        <v>1</v>
-      </c>
-      <c r="M38" s="9">
+      <c r="L38" s="7">
+        <v>1</v>
+      </c>
+      <c r="M38" s="7">
         <v>1</v>
       </c>
       <c r="N38" t="s">
@@ -3841,10 +3859,10 @@
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B39" s="8">
         <v>6039</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" t="s">
         <v>105</v>
       </c>
       <c r="D39">
@@ -3856,25 +3874,25 @@
       <c r="F39">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="7">
         <v>1.43</v>
       </c>
-      <c r="H39" s="9">
+      <c r="H39" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I39" s="12">
+      <c r="I39" s="9">
         <v>11</v>
       </c>
-      <c r="J39" s="9">
-        <v>0</v>
-      </c>
-      <c r="K39" s="9">
+      <c r="J39" s="7">
+        <v>0</v>
+      </c>
+      <c r="K39" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L39" s="9">
-        <v>1</v>
-      </c>
-      <c r="M39" s="9">
+      <c r="L39" s="7">
+        <v>1</v>
+      </c>
+      <c r="M39" s="7">
         <v>1</v>
       </c>
       <c r="N39" t="s">
@@ -3888,10 +3906,10 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="8">
         <v>6040</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" t="s">
         <v>105</v>
       </c>
       <c r="D40">
@@ -3903,25 +3921,25 @@
       <c r="F40">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="G40" s="9">
+      <c r="G40" s="7">
         <v>1.43</v>
       </c>
-      <c r="H40" s="9">
+      <c r="H40" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I40" s="12">
+      <c r="I40" s="9">
         <v>11</v>
       </c>
-      <c r="J40" s="9">
-        <v>0</v>
-      </c>
-      <c r="K40" s="9">
+      <c r="J40" s="7">
+        <v>0</v>
+      </c>
+      <c r="K40" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L40" s="9">
-        <v>1</v>
-      </c>
-      <c r="M40" s="9">
+      <c r="L40" s="7">
+        <v>1</v>
+      </c>
+      <c r="M40" s="7">
         <v>1</v>
       </c>
       <c r="N40" t="s">
@@ -3935,10 +3953,10 @@
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="10">
+      <c r="B41" s="8">
         <v>6041</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" t="s">
         <v>59</v>
       </c>
       <c r="D41">
@@ -3950,25 +3968,25 @@
       <c r="F41">
         <v>0.109</v>
       </c>
-      <c r="G41" s="9">
+      <c r="G41" s="7">
         <v>0.16</v>
       </c>
-      <c r="H41" s="9">
+      <c r="H41" s="7">
         <v>0.18</v>
       </c>
-      <c r="I41" s="12">
+      <c r="I41" s="9">
         <v>11</v>
       </c>
-      <c r="J41" s="9">
-        <v>0</v>
-      </c>
-      <c r="K41" s="9">
+      <c r="J41" s="7">
+        <v>0</v>
+      </c>
+      <c r="K41" s="7">
         <v>0.34399999999999997</v>
       </c>
-      <c r="L41" s="9">
-        <v>1</v>
-      </c>
-      <c r="M41" s="9">
+      <c r="L41" s="7">
+        <v>1</v>
+      </c>
+      <c r="M41" s="7">
         <v>1</v>
       </c>
       <c r="N41" t="s">
@@ -3982,10 +4000,10 @@
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="8">
         <v>6042</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" t="s">
         <v>62</v>
       </c>
       <c r="D42">
@@ -3997,25 +4015,25 @@
       <c r="F42">
         <v>1.9E-2</v>
       </c>
-      <c r="G42" s="9">
+      <c r="G42" s="7">
         <v>1.43</v>
       </c>
-      <c r="H42" s="9">
+      <c r="H42" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I42" s="12">
+      <c r="I42" s="9">
         <v>11</v>
       </c>
-      <c r="J42" s="9">
-        <v>0</v>
-      </c>
-      <c r="K42" s="9">
+      <c r="J42" s="7">
+        <v>0</v>
+      </c>
+      <c r="K42" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L42" s="9">
-        <v>1</v>
-      </c>
-      <c r="M42" s="9">
+      <c r="L42" s="7">
+        <v>1</v>
+      </c>
+      <c r="M42" s="7">
         <v>1</v>
       </c>
       <c r="N42" t="s">
@@ -4029,10 +4047,10 @@
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" t="s">
         <v>102</v>
       </c>
       <c r="D43">
@@ -4044,25 +4062,25 @@
       <c r="F43">
         <v>0.14799999999999999</v>
       </c>
-      <c r="G43" s="9">
+      <c r="G43" s="7">
         <v>0.48299999999999998</v>
       </c>
-      <c r="H43" s="9">
+      <c r="H43" s="7">
         <v>7.8E-2</v>
       </c>
-      <c r="I43" s="12">
+      <c r="I43" s="9">
         <v>11</v>
       </c>
-      <c r="J43" s="9">
-        <v>0</v>
-      </c>
-      <c r="K43" s="9">
+      <c r="J43" s="7">
+        <v>0</v>
+      </c>
+      <c r="K43" s="7">
         <v>0.184</v>
       </c>
-      <c r="L43" s="9">
-        <v>1</v>
-      </c>
-      <c r="M43" s="9">
+      <c r="L43" s="7">
+        <v>1</v>
+      </c>
+      <c r="M43" s="7">
         <v>1</v>
       </c>
       <c r="N43" t="s">
@@ -4079,10 +4097,10 @@
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="10">
+      <c r="B44" s="8">
         <v>6035</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" t="s">
         <v>65</v>
       </c>
       <c r="D44">
@@ -4094,25 +4112,25 @@
       <c r="F44">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G44" s="9">
+      <c r="G44" s="7">
         <v>1.43</v>
       </c>
-      <c r="H44" s="9">
+      <c r="H44" s="7">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I44" s="12">
+      <c r="I44" s="9">
         <v>11</v>
       </c>
-      <c r="J44" s="9">
-        <v>0</v>
-      </c>
-      <c r="K44" s="9">
+      <c r="J44" s="7">
+        <v>0</v>
+      </c>
+      <c r="K44" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L44" s="9">
-        <v>1</v>
-      </c>
-      <c r="M44" s="9">
+      <c r="L44" s="7">
+        <v>1</v>
+      </c>
+      <c r="M44" s="7">
         <v>1</v>
       </c>
       <c r="N44" t="s">
@@ -4126,10 +4144,10 @@
       <c r="A45" s="2">
         <v>43</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B45" s="8">
         <v>6036</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" t="s">
         <v>112</v>
       </c>
       <c r="D45">
@@ -4141,25 +4159,25 @@
       <c r="F45">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="G45" s="9">
+      <c r="G45" s="7">
         <v>2.27</v>
       </c>
-      <c r="H45" s="9">
+      <c r="H45" s="7">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="I45" s="12">
+      <c r="I45" s="9">
         <v>11</v>
       </c>
-      <c r="J45" s="9">
-        <v>0</v>
-      </c>
-      <c r="K45" s="9">
+      <c r="J45" s="7">
+        <v>0</v>
+      </c>
+      <c r="K45" s="7">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="L45" s="9">
-        <v>1</v>
-      </c>
-      <c r="M45" s="9">
+      <c r="L45" s="7">
+        <v>1</v>
+      </c>
+      <c r="M45" s="7">
         <v>1</v>
       </c>
       <c r="N45" t="s">
@@ -4232,10 +4250,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4243,7 +4261,7 @@
     <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4277,8 +4295,11 @@
       <c r="L1" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="M1" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4288,7 +4309,7 @@
       <c r="C2">
         <v>30</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="10">
         <v>7.6210000000000002E-3</v>
       </c>
       <c r="E2">
@@ -4312,8 +4333,11 @@
       <c r="L2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4323,7 +4347,7 @@
       <c r="C3">
         <v>34</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="10">
         <v>7.6210000000000002E-3</v>
       </c>
       <c r="E3">
@@ -4346,6 +4370,9 @@
       </c>
       <c r="L3" t="s">
         <v>125</v>
+      </c>
+      <c r="M3" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -4357,8 +4384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4401,7 +4428,7 @@
       <c r="L1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="6" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4415,7 +4442,7 @@
       <c r="C2">
         <v>32</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="10">
         <v>5.9760000000000004E-3</v>
       </c>
       <c r="E2">
@@ -4450,7 +4477,7 @@
       <c r="C3">
         <v>30</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="10">
         <v>7.6210000000000002E-3</v>
       </c>
       <c r="E3">
@@ -4488,7 +4515,7 @@
       <c r="C4">
         <v>24</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="10">
         <v>5.9760000000000004E-3</v>
       </c>
       <c r="E4">
@@ -4523,7 +4550,7 @@
       <c r="C5">
         <v>17</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="10">
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="E5">
@@ -4558,7 +4585,7 @@
       <c r="C6">
         <v>21</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="10">
         <v>6.6E-3</v>
       </c>
       <c r="E6">
@@ -4593,7 +4620,7 @@
       <c r="C7">
         <v>22</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="10">
         <v>9.9590000000000008E-3</v>
       </c>
       <c r="E7">
@@ -4628,7 +4655,7 @@
       <c r="C8">
         <v>33</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="10">
         <v>5.9760000000000004E-3</v>
       </c>
       <c r="E8">
@@ -4663,7 +4690,7 @@
       <c r="C9">
         <v>23</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="10">
         <v>9.5259999999999997E-3</v>
       </c>
       <c r="E9">
@@ -4698,7 +4725,7 @@
       <c r="C10">
         <v>16</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="10">
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="E10">
@@ -4733,7 +4760,7 @@
       <c r="C11">
         <v>43</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="10">
         <v>5.7499999999999999E-3</v>
       </c>
       <c r="E11">
@@ -4768,7 +4795,7 @@
       <c r="C12">
         <v>15</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="10">
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="E12">
@@ -4803,7 +4830,7 @@
       <c r="C13">
         <v>26</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="10">
         <v>1.9918999999999999E-2</v>
       </c>
       <c r="E13">
@@ -4838,7 +4865,7 @@
       <c r="C14">
         <v>26</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="10">
         <v>1.9918999999999999E-2</v>
       </c>
       <c r="E14">
@@ -4873,7 +4900,7 @@
       <c r="C15">
         <v>42</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="10">
         <v>9.9590000000000008E-3</v>
       </c>
       <c r="E15">
@@ -4908,7 +4935,7 @@
       <c r="C16">
         <v>27</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="10">
         <v>9.9590000000000008E-3</v>
       </c>
       <c r="E16">
@@ -4943,7 +4970,7 @@
       <c r="C17">
         <v>25</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="10">
         <v>7.6210000000000002E-3</v>
       </c>
       <c r="E17">
@@ -4978,7 +5005,7 @@
       <c r="C18">
         <v>18</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="10">
         <v>3.9839999999999997E-3</v>
       </c>
       <c r="E18">
@@ -5013,7 +5040,7 @@
       <c r="C19">
         <v>41</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="10">
         <v>5.7499999999999999E-3</v>
       </c>
       <c r="E19">
@@ -5048,7 +5075,7 @@
       <c r="C20">
         <v>37</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="10">
         <v>6.8999999999999999E-3</v>
       </c>
       <c r="E20">
@@ -5083,7 +5110,7 @@
       <c r="C21">
         <v>40</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="10">
         <v>5.7499999999999999E-3</v>
       </c>
       <c r="E21">
@@ -5118,7 +5145,7 @@
       <c r="C22">
         <v>36</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="10">
         <v>6.6E-3</v>
       </c>
       <c r="E22">
@@ -5153,7 +5180,7 @@
       <c r="C23">
         <v>20</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="10">
         <v>5.7499999999999999E-3</v>
       </c>
       <c r="E23">
@@ -5188,7 +5215,7 @@
       <c r="C24">
         <v>19</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="10">
         <v>6.6E-3</v>
       </c>
       <c r="E24">
@@ -5223,7 +5250,7 @@
       <c r="C25">
         <v>28</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="10">
         <v>7.6210000000000002E-3</v>
       </c>
       <c r="E25">
@@ -5258,7 +5285,7 @@
       <c r="C26">
         <v>38</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="10">
         <v>9.1999999999999998E-3</v>
       </c>
       <c r="E26">
@@ -5293,7 +5320,7 @@
       <c r="C27">
         <v>39</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="10">
         <v>5.7499999999999999E-3</v>
       </c>
       <c r="E27">
@@ -5328,7 +5355,7 @@
       <c r="C28">
         <v>29</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28" s="10">
         <v>6.8999999999999999E-3</v>
       </c>
       <c r="E28">
@@ -5363,7 +5390,7 @@
       <c r="C29">
         <v>31</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="10">
         <v>7.6210000000000002E-3</v>
       </c>
       <c r="E29">
@@ -5398,7 +5425,7 @@
       <c r="C30">
         <v>34</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="10">
         <v>7.6210000000000002E-3</v>
       </c>
       <c r="E30">
@@ -5436,7 +5463,7 @@
       <c r="C31">
         <v>35</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="10">
         <v>9.5259999999999997E-3</v>
       </c>
       <c r="E31">
@@ -5668,10 +5695,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5702,7 +5729,7 @@
       <c r="C2">
         <v>41.806010007366297</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -5714,7 +5741,7 @@
       <c r="C3">
         <v>41.806015527745622</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -6198,6 +6225,17 @@
       </c>
       <c r="C47">
         <v>41.80770972692752</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>2.2614299999999998</v>
+      </c>
+      <c r="C48">
+        <v>41.805610000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>